<commit_message>
Polarized Cap comment update
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Altium Projects\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EAB079A-5BB9-4C74-A82B-E6B919AFD7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048107DB-C72B-4A29-9AF2-BFC027DA32A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5475" yWindow="1425" windowWidth="21600" windowHeight="11475" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resistors_SMD" sheetId="1" r:id="rId1"/>
@@ -528,9 +528,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L171"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A134" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7433,9 +7433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E1AF6E3-E00B-4FA8-802B-A00B294F4270}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7604,7 +7604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA36BAAE-5FE9-424E-8D89-1CB5242DC37E}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G18" sqref="G18"/>
     </sheetView>

</xml_diff>

<commit_message>
Added TI TL072CDR OpAmp
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Altium Projects\_LIBS\GOST_Lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AA613D-1B6F-4BB5-80DA-149396BB4405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9836D8-1405-44D7-8C95-C12592DBD6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD Resistors" sheetId="1" r:id="rId1"/>
@@ -32,6 +32,7 @@
     <sheet name="Diodes" sheetId="17" r:id="rId17"/>
     <sheet name="РЭС15" sheetId="18" r:id="rId18"/>
     <sheet name="SQP Res" sheetId="19" r:id="rId19"/>
+    <sheet name="OpAmps" sheetId="20" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2685" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2697" uniqueCount="267">
   <si>
     <t>Part Number</t>
   </si>
@@ -863,6 +864,18 @@
   </si>
   <si>
     <t>SQP.PcbLib</t>
+  </si>
+  <si>
+    <t>TL072CDR</t>
+  </si>
+  <si>
+    <t>OpAmps.SchLib</t>
+  </si>
+  <si>
+    <t>SO Package.PcbLib</t>
+  </si>
+  <si>
+    <t>SO-8</t>
   </si>
 </sst>
 </file>
@@ -10489,7 +10502,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10664,6 +10677,69 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90E4213-4995-4D51-9659-5C272360332C}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" t="s">
+        <v>264</v>
+      </c>
+      <c r="E2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10990,7 +11066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80583BE-6DA8-447C-BA68-380D36F64E65}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>

</xml_diff>

<commit_message>
Added: TO-220 RLB JRB
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Altium Projects\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9836D8-1405-44D7-8C95-C12592DBD6FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7596427-76E7-4023-8695-165C9427B5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD Resistors" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,9 @@
     <sheet name="РЭС15" sheetId="18" r:id="rId18"/>
     <sheet name="SQP Res" sheetId="19" r:id="rId19"/>
     <sheet name="OpAmps" sheetId="20" r:id="rId20"/>
+    <sheet name="Analog ICs" sheetId="21" r:id="rId21"/>
+    <sheet name="RLB Inductors" sheetId="22" r:id="rId22"/>
+    <sheet name="El Cap" sheetId="23" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2697" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2754" uniqueCount="287">
   <si>
     <t>Part Number</t>
   </si>
@@ -876,6 +879,66 @@
   </si>
   <si>
     <t>SO-8</t>
+  </si>
+  <si>
+    <t>NE555DR</t>
+  </si>
+  <si>
+    <t>Analog Ics.SchLib</t>
+  </si>
+  <si>
+    <t>1N5404</t>
+  </si>
+  <si>
+    <t>DO Package.PcbLib</t>
+  </si>
+  <si>
+    <t>DO-201AD</t>
+  </si>
+  <si>
+    <t>RLB.PcbLib</t>
+  </si>
+  <si>
+    <t>RLB0914</t>
+  </si>
+  <si>
+    <t>1000мк</t>
+  </si>
+  <si>
+    <t>RLB0914-102KL</t>
+  </si>
+  <si>
+    <t>Voltage</t>
+  </si>
+  <si>
+    <t>ECAP (К50-35)</t>
+  </si>
+  <si>
+    <t>JRB.PcbLib</t>
+  </si>
+  <si>
+    <t>22мк</t>
+  </si>
+  <si>
+    <t>350В</t>
+  </si>
+  <si>
+    <t>JRB12.5/13</t>
+  </si>
+  <si>
+    <t>STP11NK50Z</t>
+  </si>
+  <si>
+    <t>TO-220</t>
+  </si>
+  <si>
+    <t>500В</t>
+  </si>
+  <si>
+    <t>10А</t>
+  </si>
+  <si>
+    <t>0,48Ом</t>
   </si>
 </sst>
 </file>
@@ -10326,20 +10389,23 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DFAC1-75D7-46B3-9775-134B736AC5F9}">
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10347,7 +10413,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>84</v>
+        <v>253</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
@@ -10427,6 +10493,26 @@
       </c>
       <c r="K3" t="s">
         <v>245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" t="s">
+        <v>269</v>
+      </c>
+      <c r="C4" t="s">
+        <v>247</v>
+      </c>
+      <c r="D4" t="s">
+        <v>271</v>
+      </c>
+      <c r="J4" t="s">
+        <v>243</v>
+      </c>
+      <c r="K4" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -10685,8 +10771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90E4213-4995-4D51-9659-5C272360332C}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10737,6 +10823,216 @@
       </c>
       <c r="F2" t="s">
         <v>263</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF9B95B-134C-4FD8-8A48-B6718728E3BB}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" t="s">
+        <v>268</v>
+      </c>
+      <c r="E2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3FA756-703C-41CB-92CC-596399589CC9}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>272</v>
+      </c>
+      <c r="F2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CADBAED-E8E5-4970-8DAA-34238D39F5D0}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>281</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F2" t="s">
+        <v>277</v>
+      </c>
+      <c r="G2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H2" t="s">
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -11064,11 +11360,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80583BE-6DA8-447C-BA68-380D36F64E65}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11243,6 +11539,35 @@
       </c>
       <c r="Q7" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I8" t="s">
+        <v>61</v>
+      </c>
+      <c r="J8" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" t="s">
+        <v>284</v>
+      </c>
+      <c r="L8" t="s">
+        <v>285</v>
+      </c>
+      <c r="M8" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>282</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added: Potentiometer Core Inductors Voltage Reference DAC OpAmp
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Altium Projects\_LIBS\GOST_Lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7596427-76E7-4023-8695-165C9427B5CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6198DBCA-6F39-4256-8667-9B6465B8ED36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="15" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD Resistors" sheetId="1" r:id="rId1"/>
@@ -36,6 +36,9 @@
     <sheet name="Analog ICs" sheetId="21" r:id="rId21"/>
     <sheet name="RLB Inductors" sheetId="22" r:id="rId22"/>
     <sheet name="El Cap" sheetId="23" r:id="rId23"/>
+    <sheet name="Potentiometers" sheetId="24" r:id="rId24"/>
+    <sheet name="DACs" sheetId="25" r:id="rId25"/>
+    <sheet name="Voltage Reference" sheetId="26" r:id="rId26"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2754" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2816" uniqueCount="308">
   <si>
     <t>Part Number</t>
   </si>
@@ -939,6 +942,69 @@
   </si>
   <si>
     <t>0,48Ом</t>
+  </si>
+  <si>
+    <t>RLB1314</t>
+  </si>
+  <si>
+    <t>RLB1314-221KL</t>
+  </si>
+  <si>
+    <t>220мк</t>
+  </si>
+  <si>
+    <t>BC817</t>
+  </si>
+  <si>
+    <t>Structure</t>
+  </si>
+  <si>
+    <t>N-ch</t>
+  </si>
+  <si>
+    <t>NPN</t>
+  </si>
+  <si>
+    <t>BJT-NPN-BEC</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>3266W-1-101LF</t>
+  </si>
+  <si>
+    <t>RES HOLE.PcbLib</t>
+  </si>
+  <si>
+    <t>3266W</t>
+  </si>
+  <si>
+    <t>OpAmp 8Pin</t>
+  </si>
+  <si>
+    <t>SOIC-8</t>
+  </si>
+  <si>
+    <t>LM6172IM/NOPB</t>
+  </si>
+  <si>
+    <t>AD5542BRZ</t>
+  </si>
+  <si>
+    <t>SOIC-14</t>
+  </si>
+  <si>
+    <t>Bits</t>
+  </si>
+  <si>
+    <t>DACs.SchLib</t>
+  </si>
+  <si>
+    <t>LM285Z-2.5/NOPB</t>
+  </si>
+  <si>
+    <t>Zener-AC</t>
   </si>
 </sst>
 </file>
@@ -10769,20 +10835,20 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90E4213-4995-4D51-9659-5C272360332C}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -10810,7 +10876,7 @@
         <v>263</v>
       </c>
       <c r="B2" t="s">
-        <v>263</v>
+        <v>299</v>
       </c>
       <c r="C2" t="s">
         <v>266</v>
@@ -10823,6 +10889,26 @@
       </c>
       <c r="F2" t="s">
         <v>263</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>301</v>
+      </c>
+      <c r="B3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D3" t="s">
+        <v>264</v>
+      </c>
+      <c r="E3" t="s">
+        <v>265</v>
+      </c>
+      <c r="F3" t="s">
+        <v>301</v>
       </c>
     </row>
   </sheetData>
@@ -10895,10 +10981,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C3FA756-703C-41CB-92CC-596399589CC9}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10958,6 +11044,29 @@
         <v>274</v>
       </c>
     </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" t="s">
+        <v>272</v>
+      </c>
+      <c r="F3" t="s">
+        <v>288</v>
+      </c>
+      <c r="G3" t="s">
+        <v>289</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10969,7 +11078,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11003,7 +11112,7 @@
         <v>253</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>276</v>
@@ -11033,6 +11142,215 @@
       </c>
       <c r="H2" t="s">
         <v>280</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB034B99-E4EF-41D8-8723-B0F620C49749}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>296</v>
+      </c>
+      <c r="B2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C2" t="s">
+        <v>298</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16020252-59AC-4E88-B695-96D3C1364171}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D2" t="s">
+        <v>305</v>
+      </c>
+      <c r="E2" t="s">
+        <v>265</v>
+      </c>
+      <c r="F2" t="s">
+        <v>302</v>
+      </c>
+      <c r="G2">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8C0CC4-DB37-42CD-B200-C3A1775B2B6D}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" t="s">
+        <v>306</v>
+      </c>
+      <c r="G2">
+        <v>2.5</v>
       </c>
     </row>
   </sheetData>
@@ -11360,11 +11678,11 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80583BE-6DA8-447C-BA68-380D36F64E65}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomLeft" activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11406,7 +11724,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>9</v>
+        <v>291</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
@@ -11493,6 +11811,9 @@
       <c r="C6" t="s">
         <v>66</v>
       </c>
+      <c r="H6" t="s">
+        <v>292</v>
+      </c>
       <c r="I6" t="s">
         <v>61</v>
       </c>
@@ -11531,6 +11852,9 @@
       <c r="C7" t="s">
         <v>258</v>
       </c>
+      <c r="H7" t="s">
+        <v>292</v>
+      </c>
       <c r="I7" t="s">
         <v>61</v>
       </c>
@@ -11551,6 +11875,9 @@
       <c r="C8" t="s">
         <v>283</v>
       </c>
+      <c r="H8" t="s">
+        <v>292</v>
+      </c>
       <c r="I8" t="s">
         <v>61</v>
       </c>
@@ -11568,6 +11895,26 @@
       </c>
       <c r="Q8" t="s">
         <v>282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>290</v>
+      </c>
+      <c r="B9" t="s">
+        <v>294</v>
+      </c>
+      <c r="C9" t="s">
+        <v>258</v>
+      </c>
+      <c r="H9" t="s">
+        <v>293</v>
+      </c>
+      <c r="I9" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added: ElCAP 3D Model Voltage Invertor
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6198DBCA-6F39-4256-8667-9B6465B8ED36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A2E8581-A1ED-4C54-A2ED-A5B0E117485B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="15" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="16" activeTab="26" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD Resistors" sheetId="1" r:id="rId1"/>
@@ -39,6 +39,7 @@
     <sheet name="Potentiometers" sheetId="24" r:id="rId24"/>
     <sheet name="DACs" sheetId="25" r:id="rId25"/>
     <sheet name="Voltage Reference" sheetId="26" r:id="rId26"/>
+    <sheet name="Voltage Sources" sheetId="27" r:id="rId27"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2816" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2829" uniqueCount="311">
   <si>
     <t>Part Number</t>
   </si>
@@ -1005,6 +1006,15 @@
   </si>
   <si>
     <t>Zener-AC</t>
+  </si>
+  <si>
+    <t>TPS60403DBVR</t>
+  </si>
+  <si>
+    <t>VoltageSources.SchLib</t>
+  </si>
+  <si>
+    <t>SOT-23-5</t>
   </si>
 </sst>
 </file>
@@ -11293,8 +11303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB8C0CC4-DB37-42CD-B200-C3A1775B2B6D}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11351,6 +11361,70 @@
       </c>
       <c r="G2">
         <v>2.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15A3438-F635-42B7-BA09-618C7E84CE48}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B2" t="s">
+        <v>308</v>
+      </c>
+      <c r="C2" t="s">
+        <v>310</v>
+      </c>
+      <c r="D2" t="s">
+        <v>309</v>
+      </c>
+      <c r="E2" t="s">
+        <v>257</v>
+      </c>
+      <c r="F2" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Milandr K1986BE92QI in LQFP64 package
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D07877B-66FB-4BF7-ADB1-A2901B9D0D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AF4E29-58C5-4834-A715-2E6F19541837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="5" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="17" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD Resistors" sheetId="1" r:id="rId1"/>
@@ -40,6 +40,7 @@
     <sheet name="DACs" sheetId="25" r:id="rId25"/>
     <sheet name="Voltage Reference" sheetId="26" r:id="rId26"/>
     <sheet name="Voltage Sources" sheetId="27" r:id="rId27"/>
+    <sheet name="MCU" sheetId="28" r:id="rId28"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2846" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="324">
   <si>
     <t>Part Number</t>
   </si>
@@ -1042,6 +1043,18 @@
   </si>
   <si>
     <t>BJT-PNP-BEC</t>
+  </si>
+  <si>
+    <t>LQFP64</t>
+  </si>
+  <si>
+    <t>LQFP.PcbLib</t>
+  </si>
+  <si>
+    <t>MCU.SchLib</t>
+  </si>
+  <si>
+    <t>K1986BE92QI</t>
   </si>
 </sst>
 </file>
@@ -11400,7 +11413,7 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11452,6 +11465,62 @@
       </c>
       <c r="F2" t="s">
         <v>307</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24740AD4-1F39-4A81-B96D-3AE6D15F5B16}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>323</v>
+      </c>
+      <c r="B2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D2" t="s">
+        <v>322</v>
+      </c>
+      <c r="E2" t="s">
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -11781,7 +11850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A80583BE-6DA8-447C-BA68-380D36F64E65}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>

</xml_diff>

<commit_message>
Added CP2102 USB-UART in PQFN-28 Package Added PGB1010603MR protection diode in o603 package
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Altium Projects\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AF4E29-58C5-4834-A715-2E6F19541837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F910B7C-7606-45AE-BCF5-C6480A0B5165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="17" activeTab="27" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32715" yWindow="4215" windowWidth="24885" windowHeight="11385" firstSheet="21" activeTab="28" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD Resistors" sheetId="1" r:id="rId1"/>
@@ -41,6 +41,7 @@
     <sheet name="Voltage Reference" sheetId="26" r:id="rId26"/>
     <sheet name="Voltage Sources" sheetId="27" r:id="rId27"/>
     <sheet name="MCU" sheetId="28" r:id="rId28"/>
+    <sheet name="Converters" sheetId="29" r:id="rId29"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -61,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2874" uniqueCount="333">
   <si>
     <t>Part Number</t>
   </si>
@@ -1055,6 +1056,33 @@
   </si>
   <si>
     <t>K1986BE92QI</t>
+  </si>
+  <si>
+    <t>PGB1010603MR</t>
+  </si>
+  <si>
+    <t>Zener-Duplex</t>
+  </si>
+  <si>
+    <t>RES_SMD.PcbLib</t>
+  </si>
+  <si>
+    <t>CP2102-GMR</t>
+  </si>
+  <si>
+    <t>PQFN-28</t>
+  </si>
+  <si>
+    <t>Converters.SchLib</t>
+  </si>
+  <si>
+    <t>QFN.PcbLib</t>
+  </si>
+  <si>
+    <t>X/Y</t>
+  </si>
+  <si>
+    <t>USB-UART</t>
   </si>
 </sst>
 </file>
@@ -10505,18 +10533,18 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DFAC1-75D7-46B3-9775-134B736AC5F9}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
@@ -10631,8 +10659,29 @@
         <v>269</v>
       </c>
     </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>324</v>
+      </c>
+      <c r="B5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C5" t="s">
+        <v>325</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" t="s">
+        <v>242</v>
+      </c>
+      <c r="K5" t="s">
+        <v>326</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11476,8 +11525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24740AD4-1F39-4A81-B96D-3AE6D15F5B16}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11521,6 +11570,69 @@
       </c>
       <c r="E2" t="s">
         <v>321</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C841E41E-3033-4328-9AAE-D6BAE19485E1}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" t="s">
+        <v>327</v>
+      </c>
+      <c r="C2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2" t="s">
+        <v>329</v>
+      </c>
+      <c r="E2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F2" t="s">
+        <v>332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ADHV4702-1 in LFCSP-12 package
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Altium Projects\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6EECD8-588B-44F7-A135-5CCB8DD5D2EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DB04BE-E6D3-4F46-863D-928EF8875D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="14" activeTab="23" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD Resistors" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2890" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="361">
   <si>
     <t>Part Number</t>
   </si>
@@ -1153,6 +1153,15 @@
   </si>
   <si>
     <t>16 MHz</t>
+  </si>
+  <si>
+    <t>ADHV4702-1</t>
+  </si>
+  <si>
+    <t>LFCSP.PcbLib</t>
+  </si>
+  <si>
+    <t>LFCSP-12</t>
   </si>
 </sst>
 </file>
@@ -9371,10 +9380,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90E4213-4995-4D51-9659-5C272360332C}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9445,6 +9454,26 @@
       </c>
       <c r="F3" t="s">
         <v>299</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>358</v>
+      </c>
+      <c r="B4" t="s">
+        <v>358</v>
+      </c>
+      <c r="C4" t="s">
+        <v>360</v>
+      </c>
+      <c r="D4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" t="s">
+        <v>359</v>
+      </c>
+      <c r="F4" t="s">
+        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -10195,7 +10224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B82A66D0-2486-4B81-8612-E82AD24841A3}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
bugfix Added Schottky double diode
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Altium Projects\_LIBS\GOST_Lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DB04BE-E6D3-4F46-863D-928EF8875D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EAA712-6607-4639-9451-0CDDD6030D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="11" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5985" yWindow="3345" windowWidth="21600" windowHeight="11475" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD Resistors" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2896" uniqueCount="361">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2901" uniqueCount="366">
   <si>
     <t>Part Number</t>
   </si>
@@ -1162,6 +1162,21 @@
   </si>
   <si>
     <t>LFCSP-12</t>
+  </si>
+  <si>
+    <t>BAS70-04</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Dual Schottky</t>
+  </si>
+  <si>
+    <t>DoubleSchottky-AC</t>
+  </si>
+  <si>
+    <t>ECAP (К50-35) 22мк</t>
   </si>
 </sst>
 </file>
@@ -9040,26 +9055,26 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DFAC1-75D7-46B3-9775-134B736AC5F9}">
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9076,43 +9091,34 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>362</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>9</v>
+        <v>74</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>2</v>
+        <v>75</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q1" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>240</v>
       </c>
@@ -9122,11 +9128,11 @@
       <c r="C2" t="s">
         <v>245</v>
       </c>
-      <c r="J2" t="s">
+      <c r="G2" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>242</v>
       </c>
@@ -9139,14 +9145,14 @@
       <c r="D3" t="s">
         <v>244</v>
       </c>
-      <c r="J3" t="s">
+      <c r="G3" t="s">
         <v>241</v>
       </c>
-      <c r="K3" t="s">
+      <c r="H3" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>267</v>
       </c>
@@ -9159,14 +9165,14 @@
       <c r="D4" t="s">
         <v>269</v>
       </c>
-      <c r="J4" t="s">
+      <c r="G4" t="s">
         <v>241</v>
       </c>
-      <c r="K4" t="s">
+      <c r="H4" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>323</v>
       </c>
@@ -9179,14 +9185,14 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-      <c r="J5" t="s">
+      <c r="G5" t="s">
         <v>241</v>
       </c>
-      <c r="K5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>334</v>
       </c>
@@ -9196,8 +9202,31 @@
       <c r="C6" t="s">
         <v>335</v>
       </c>
-      <c r="J6" t="s">
+      <c r="G6" t="s">
         <v>241</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>361</v>
+      </c>
+      <c r="B7" t="s">
+        <v>361</v>
+      </c>
+      <c r="C7" t="s">
+        <v>364</v>
+      </c>
+      <c r="D7" t="s">
+        <v>256</v>
+      </c>
+      <c r="F7" t="s">
+        <v>363</v>
+      </c>
+      <c r="G7" t="s">
+        <v>241</v>
+      </c>
+      <c r="H7" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -9383,7 +9412,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9643,7 +9672,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9653,7 +9682,7 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9700,7 +9729,7 @@
         <v>276</v>
       </c>
       <c r="F2" t="s">
-        <v>275</v>
+        <v>365</v>
       </c>
       <c r="G2" t="s">
         <v>277</v>
@@ -9856,11 +9885,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4164A9E-FF46-467E-B380-FA61312CCDD8}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
+      <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9871,10 +9900,10 @@
     <col min="4" max="11" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9915,10 +9944,13 @@
         <v>3</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -9959,6 +9991,9 @@
         <v>63</v>
       </c>
       <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bugfixes Added 3D models for SQP 10W Resistors an РЭС15 Relays
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EAA712-6607-4639-9451-0CDDD6030D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0516F9B-5125-4ED9-8307-3C254CE56A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5985" yWindow="3345" windowWidth="21600" windowHeight="11475" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5985" yWindow="3345" windowWidth="21600" windowHeight="11475" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD Resistors" sheetId="1" r:id="rId1"/>
@@ -9239,7 +9239,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1047152A-FCBE-403C-A91A-439AB27AC722}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -9411,7 +9411,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90E4213-4995-4D51-9659-5C272360332C}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Diode bridge, Zenner 18V
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Altium\AD21\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0516F9B-5125-4ED9-8307-3C254CE56A59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B955330-8FE5-44FD-8BE5-2C4A23368EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5985" yWindow="3345" windowWidth="21600" windowHeight="11475" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" firstSheet="9" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD Resistors" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2901" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2928" uniqueCount="381">
   <si>
     <t>Part Number</t>
   </si>
@@ -906,9 +906,6 @@
     <t>Voltage</t>
   </si>
   <si>
-    <t>ECAP (К50-35)</t>
-  </si>
-  <si>
     <t>JRB.PcbLib</t>
   </si>
   <si>
@@ -1177,6 +1174,54 @@
   </si>
   <si>
     <t>ECAP (К50-35) 22мк</t>
+  </si>
+  <si>
+    <t>AD620</t>
+  </si>
+  <si>
+    <t>ОУ</t>
+  </si>
+  <si>
+    <t>Инструментальный</t>
+  </si>
+  <si>
+    <t>Bridge</t>
+  </si>
+  <si>
+    <t>WOG</t>
+  </si>
+  <si>
+    <t>WOG Package.PcbLib</t>
+  </si>
+  <si>
+    <t>2W10G-E4/51</t>
+  </si>
+  <si>
+    <t>Zener-CA</t>
+  </si>
+  <si>
+    <t>MiniMELF/SOD80</t>
+  </si>
+  <si>
+    <t>MELF Package.PcbLib</t>
+  </si>
+  <si>
+    <t>BZV55C18</t>
+  </si>
+  <si>
+    <t>Zener 18V</t>
+  </si>
+  <si>
+    <t>400В</t>
+  </si>
+  <si>
+    <t>100мк</t>
+  </si>
+  <si>
+    <t>ECAP (К50-35) 100мк</t>
+  </si>
+  <si>
+    <t>JRB18</t>
   </si>
 </sst>
 </file>
@@ -8964,7 +9009,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>17</v>
@@ -9001,16 +9046,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E3" t="s">
         <v>235</v>
@@ -9021,13 +9066,13 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E4" t="s">
         <v>235</v>
@@ -9035,13 +9080,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>349</v>
+      </c>
+      <c r="B5" t="s">
         <v>350</v>
       </c>
-      <c r="B5" t="s">
-        <v>351</v>
-      </c>
       <c r="C5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E5" t="s">
         <v>235</v>
@@ -9055,26 +9100,25 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DFAC1-75D7-46B3-9775-134B736AC5F9}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9091,7 +9135,7 @@
         <v>5</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
@@ -9099,26 +9143,8 @@
       <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>240</v>
       </c>
@@ -9132,7 +9158,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>242</v>
       </c>
@@ -9152,7 +9178,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>267</v>
       </c>
@@ -9172,15 +9198,15 @@
         <v>268</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>322</v>
+      </c>
+      <c r="B5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C5" t="s">
         <v>323</v>
-      </c>
-      <c r="B5" t="s">
-        <v>323</v>
-      </c>
-      <c r="C5" t="s">
-        <v>324</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -9192,41 +9218,87 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>333</v>
+      </c>
+      <c r="B6" t="s">
+        <v>333</v>
+      </c>
+      <c r="C6" t="s">
         <v>334</v>
-      </c>
-      <c r="B6" t="s">
-        <v>334</v>
-      </c>
-      <c r="C6" t="s">
-        <v>335</v>
       </c>
       <c r="G6" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D7" t="s">
         <v>256</v>
       </c>
       <c r="F7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G7" t="s">
         <v>241</v>
       </c>
       <c r="H7" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>371</v>
+      </c>
+      <c r="B8" t="s">
+        <v>371</v>
+      </c>
+      <c r="C8" t="s">
+        <v>368</v>
+      </c>
+      <c r="D8" t="s">
+        <v>369</v>
+      </c>
+      <c r="F8" t="s">
+        <v>368</v>
+      </c>
+      <c r="G8" t="s">
+        <v>241</v>
+      </c>
+      <c r="H8" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>375</v>
+      </c>
+      <c r="B9" t="s">
+        <v>375</v>
+      </c>
+      <c r="C9" t="s">
+        <v>372</v>
+      </c>
+      <c r="D9" t="s">
+        <v>373</v>
+      </c>
+      <c r="F9" t="s">
+        <v>376</v>
+      </c>
+      <c r="G9" t="s">
+        <v>241</v>
+      </c>
+      <c r="H9" t="s">
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -9239,7 +9311,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1047152A-FCBE-403C-A91A-439AB27AC722}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -9409,10 +9481,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F90E4213-4995-4D51-9659-5C272360332C}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9423,9 +9495,10 @@
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9444,13 +9517,16 @@
       <c r="F1" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>261</v>
       </c>
       <c r="B2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C2" t="s">
         <v>264</v>
@@ -9464,16 +9540,19 @@
       <c r="F2" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C3" t="s">
         <v>297</v>
-      </c>
-      <c r="C3" t="s">
-        <v>298</v>
       </c>
       <c r="D3" t="s">
         <v>262</v>
@@ -9482,27 +9561,56 @@
         <v>263</v>
       </c>
       <c r="F3" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+      <c r="G3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="D4" t="s">
         <v>262</v>
       </c>
       <c r="E4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F4" t="s">
-        <v>358</v>
+        <v>357</v>
+      </c>
+      <c r="G4" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B5" t="s">
+        <v>365</v>
+      </c>
+      <c r="C5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D5" t="s">
+        <v>262</v>
+      </c>
+      <c r="E5" t="s">
+        <v>263</v>
+      </c>
+      <c r="F5" t="s">
+        <v>365</v>
+      </c>
+      <c r="G5" t="s">
+        <v>367</v>
       </c>
     </row>
   </sheetData>
@@ -9640,13 +9748,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B3" t="s">
         <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D3" t="s">
         <v>42</v>
@@ -9655,10 +9763,10 @@
         <v>270</v>
       </c>
       <c r="F3" t="s">
+        <v>285</v>
+      </c>
+      <c r="G3" t="s">
         <v>286</v>
-      </c>
-      <c r="G3" t="s">
-        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -9669,20 +9777,20 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CADBAED-E8E5-4970-8DAA-34238D39F5D0}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9714,28 +9822,54 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>275</v>
+        <v>364</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
       </c>
       <c r="E2" t="s">
+        <v>275</v>
+      </c>
+      <c r="F2" t="s">
+        <v>364</v>
+      </c>
+      <c r="G2" t="s">
         <v>276</v>
       </c>
-      <c r="F2" t="s">
-        <v>365</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>277</v>
       </c>
-      <c r="H2" t="s">
-        <v>278</v>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>380</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>275</v>
+      </c>
+      <c r="F3" t="s">
+        <v>379</v>
+      </c>
+      <c r="G3" t="s">
+        <v>378</v>
+      </c>
+      <c r="H3" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -9789,22 +9923,22 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>294</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>293</v>
-      </c>
-      <c r="C2" t="s">
-        <v>296</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>295</v>
-      </c>
-      <c r="F2" t="s">
-        <v>294</v>
       </c>
       <c r="G2">
         <v>100</v>
@@ -9852,27 +9986,27 @@
         <v>251</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" t="s">
+        <v>299</v>
+      </c>
+      <c r="C2" t="s">
         <v>300</v>
       </c>
-      <c r="B2" t="s">
-        <v>300</v>
-      </c>
-      <c r="C2" t="s">
-        <v>301</v>
-      </c>
       <c r="D2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E2" t="s">
         <v>263</v>
       </c>
       <c r="F2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G2">
         <v>16</v>
@@ -10046,10 +10180,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>303</v>
+      </c>
+      <c r="B2" t="s">
         <v>304</v>
-      </c>
-      <c r="B2" t="s">
-        <v>305</v>
       </c>
       <c r="C2" t="s">
         <v>66</v>
@@ -10061,7 +10195,7 @@
         <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G2">
         <v>2.5</v>
@@ -10113,22 +10247,22 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D2" t="s">
         <v>306</v>
-      </c>
-      <c r="B2" t="s">
-        <v>306</v>
-      </c>
-      <c r="C2" t="s">
-        <v>308</v>
-      </c>
-      <c r="D2" t="s">
-        <v>307</v>
       </c>
       <c r="E2" t="s">
         <v>255</v>
       </c>
       <c r="F2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -10172,19 +10306,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C2" t="s">
+        <v>318</v>
+      </c>
+      <c r="D2" t="s">
+        <v>320</v>
+      </c>
+      <c r="E2" t="s">
         <v>319</v>
-      </c>
-      <c r="D2" t="s">
-        <v>321</v>
-      </c>
-      <c r="E2" t="s">
-        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -10227,27 +10361,27 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" t="s">
+        <v>324</v>
+      </c>
+      <c r="C2" t="s">
         <v>325</v>
       </c>
-      <c r="B2" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>326</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>327</v>
       </c>
-      <c r="E2" t="s">
-        <v>328</v>
-      </c>
       <c r="F2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
   </sheetData>
@@ -10295,30 +10429,30 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>351</v>
+      </c>
+      <c r="B2" t="s">
         <v>352</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>353</v>
       </c>
-      <c r="D2" t="s">
-        <v>354</v>
-      </c>
       <c r="F2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B3" t="s">
+        <v>352</v>
+      </c>
+      <c r="D3" t="s">
         <v>353</v>
       </c>
-      <c r="D3" t="s">
-        <v>354</v>
-      </c>
       <c r="F3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -10692,7 +10826,7 @@
         <v>8</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>2</v>
@@ -10780,7 +10914,7 @@
         <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I6" t="s">
         <v>61</v>
@@ -10789,7 +10923,7 @@
         <v>65</v>
       </c>
       <c r="K6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="L6" t="s">
         <v>76</v>
@@ -10821,7 +10955,7 @@
         <v>256</v>
       </c>
       <c r="H7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I7" t="s">
         <v>61</v>
@@ -10835,16 +10969,16 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B8" t="s">
         <v>83</v>
       </c>
       <c r="C8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="H8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I8" t="s">
         <v>61</v>
@@ -10853,50 +10987,50 @@
         <v>65</v>
       </c>
       <c r="K8" t="s">
+        <v>281</v>
+      </c>
+      <c r="L8" t="s">
         <v>282</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>283</v>
       </c>
-      <c r="M8" t="s">
-        <v>284</v>
-      </c>
       <c r="Q8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C9" t="s">
         <v>256</v>
       </c>
       <c r="H9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="I9" t="s">
         <v>61</v>
       </c>
       <c r="Q9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>308</v>
+      </c>
+      <c r="B10" t="s">
         <v>309</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>280</v>
+      </c>
+      <c r="H10" t="s">
         <v>310</v>
-      </c>
-      <c r="C10" t="s">
-        <v>281</v>
-      </c>
-      <c r="H10" t="s">
-        <v>311</v>
       </c>
       <c r="I10" t="s">
         <v>61</v>
@@ -10905,30 +11039,30 @@
         <v>65</v>
       </c>
       <c r="K10" t="s">
+        <v>312</v>
+      </c>
+      <c r="L10" t="s">
         <v>313</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>314</v>
       </c>
-      <c r="M10" t="s">
-        <v>315</v>
-      </c>
       <c r="Q10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C11" t="s">
         <v>256</v>
       </c>
       <c r="H11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I11" t="s">
         <v>61</v>
@@ -10937,7 +11071,7 @@
         <v>255</v>
       </c>
       <c r="Q11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -10985,22 +11119,22 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>341</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>343</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -11805,40 +11939,40 @@
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B42" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C42" t="s">
         <v>131</v>
       </c>
       <c r="D42" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E42" t="s">
         <v>68</v>
       </c>
       <c r="F42" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G42" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H42" t="s">
+        <v>345</v>
+      </c>
+      <c r="I42" t="s">
+        <v>344</v>
+      </c>
+      <c r="J42" t="s">
         <v>346</v>
       </c>
-      <c r="I42" t="s">
-        <v>345</v>
-      </c>
-      <c r="J42" t="s">
+      <c r="K42" t="s">
         <v>347</v>
       </c>
-      <c r="K42" t="s">
+      <c r="L42" t="s">
         <v>348</v>
-      </c>
-      <c r="L42" t="s">
-        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Milandr MCU module
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Altium Projects\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500D3829-37F8-42E3-B7FD-E1616139FC46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1A24BC-F028-449C-9E65-6EA50A0DA423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="15" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD Resistors" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2948" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2956" uniqueCount="392">
   <si>
     <t>Part Number</t>
   </si>
@@ -1244,6 +1244,18 @@
   </si>
   <si>
     <t>Bridge-SSPN</t>
+  </si>
+  <si>
+    <t>LDM-BB-K1986BE92QI</t>
+  </si>
+  <si>
+    <t>Modules.PcbLib</t>
+  </si>
+  <si>
+    <t>Отладочная плата</t>
+  </si>
+  <si>
+    <t>Микросхема</t>
   </si>
 </sst>
 </file>
@@ -9124,7 +9136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DFAC1-75D7-46B3-9775-134B736AC5F9}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
@@ -10385,22 +10397,21 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24740AD4-1F39-4A81-B96D-3AE6D15F5B16}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10416,8 +10427,11 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>321</v>
       </c>
@@ -10432,6 +10446,29 @@
       </c>
       <c r="E2" t="s">
         <v>319</v>
+      </c>
+      <c r="F2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B3" t="s">
+        <v>388</v>
+      </c>
+      <c r="C3" t="s">
+        <v>388</v>
+      </c>
+      <c r="D3" t="s">
+        <v>320</v>
+      </c>
+      <c r="E3" t="s">
+        <v>389</v>
+      </c>
+      <c r="F3" t="s">
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added SMD LED in 0603 Package
</commit_message>
<xml_diff>
--- a/GOST_DbLib.xlsx
+++ b/GOST_DbLib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Altium Projects\_LIBS\GOST_Lib\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE311C40-0DA7-47A4-A38C-42FB3E967123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49CDDEB-E3B2-4DC5-9EDA-6E727F7A3260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31845" yWindow="2115" windowWidth="24885" windowHeight="11385" firstSheet="8" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SMD Resistors" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2982" uniqueCount="402">
   <si>
     <t>Part Number</t>
   </si>
@@ -1277,6 +1277,15 @@
   </si>
   <si>
     <t>Schottky</t>
+  </si>
+  <si>
+    <t>LL-S194PUGC-2B</t>
+  </si>
+  <si>
+    <t>LED.PcbLib</t>
+  </si>
+  <si>
+    <t>LED 0603</t>
   </si>
 </sst>
 </file>
@@ -9174,11 +9183,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62DFAC1-75D7-46B3-9775-134B736AC5F9}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9396,6 +9405,29 @@
       </c>
       <c r="H10" t="s">
         <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>399</v>
+      </c>
+      <c r="B11" t="s">
+        <v>399</v>
+      </c>
+      <c r="C11" t="s">
+        <v>334</v>
+      </c>
+      <c r="D11" t="s">
+        <v>401</v>
+      </c>
+      <c r="F11" t="s">
+        <v>333</v>
+      </c>
+      <c r="G11" t="s">
+        <v>241</v>
+      </c>
+      <c r="H11" t="s">
+        <v>400</v>
       </c>
     </row>
   </sheetData>

</xml_diff>